<commit_message>
Add deployment configurations for multiple platforms
</commit_message>
<xml_diff>
--- a/bu_mapping_current.xlsx
+++ b/bu_mapping_current.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,12 +504,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Andrew Ngan</t>
+          <t>Apiwat</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sngan@anantaraclub.com</t>
+          <t>apiwat.s@codemonday.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -538,34 +538,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Arthit Kruewisen</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>arthit@italots.com</t>
+          <t>asukkaew@deloitte.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bobby Leong</t>
+          <t>Atiwit</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>sleong@anantaraclub.com</t>
+          <t>atiwit_wi@minor.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
@@ -589,46 +589,46 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BOY [CODEMONDAY]</t>
+          <t>Chayanon Lormanometee</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>phuwanat.t@codemonday.com</t>
+          <t>chayanon_lo@minor.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Commercial</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chandni Chawla</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>chandni_ch@anantaraclub.com</t>
+          <t>chchongchalearmpaibo@deloitte.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Chanon Sillapasunthon</t>
+          <t>Chinnawat Phutthatham</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>chanon@hypcode.co</t>
+          <t>chinnawat_ph@minor.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -640,29 +640,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chayanon Lormanometee</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>chayanon_lo@minor.com</t>
+          <t>darchong@deloitte.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chinnawat Phutthatham</t>
+          <t>Arzion</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>chinnawat_ph@minor.com</t>
+          <t>dario.pereyra@arzion.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
@@ -701,19 +701,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>German Orlando</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>german.orlando@arzion.com</t>
+          <t>echoyan@deloitte.com.cn</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -725,12 +725,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Guido Traversaro</t>
+          <t>German Orlando</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>guido.traversaro@arzion.com</t>
+          <t>german.orlando@arzion.com</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -742,29 +742,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jaruwan Chaimanun</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>jaruwan_ch@minor.com</t>
+          <t>gteo@deloitte.com</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jasmine</t>
+          <t>Guido Traversaro</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>yyeo@anantaraclub.com</t>
+          <t>guido.traversaro@arzion.com</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -776,29 +776,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jill Ji</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>jiji@minor.com</t>
+          <t>jduangjaidee@deloitte.com</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Job [CODEMONDAY]</t>
+          <t>Jill Ji</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>patchanop.l@codemonday.com</t>
+          <t>jiji@minor.com</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,80 +810,80 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Joshua Rey Nicolie Cordero</t>
+          <t>Kamonchanok S.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>jcordero@minor.com</t>
+          <t>kamonchanok_si@minor.com</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>FS</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Kamonchanok S.</t>
+          <t>Khemmanij Tansui</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>kamonchanok_si@minor.com</t>
+          <t>khemmanij_ta@minor.com</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Khemmanij Tansui</t>
+          <t>Khongsak Kawdettikhun</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>khemmanij_ta@minor.com</t>
+          <t>khongsak@hypcode.co</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Khongsak Kawdettikhun</t>
+          <t>Kitti Tongpraduppet</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>khongsak@hypcode.co</t>
+          <t>kitti.tongpraduppet@gmail.com</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Kitti Tongpraduppet</t>
+          <t>Kittipong Balang</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>kitti.tongpraduppet@gmail.com</t>
+          <t>kittipong_ba@minor.com</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -895,17 +895,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Kittipong Balang</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>kittipong_ba@minor.com</t>
+          <t>kkositanont@deloitte.com</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
@@ -922,87 +922,87 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mat√≠as Uhart</t>
+          <t>Lamai - Contract Admin</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>matias.uhart@kognitiv.com</t>
+          <t>lamai_nu@minor.com</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mongkol Kanaworrakul</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>mongkol@italots.com</t>
+          <t>mingsun@deloitte.com.cn</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Nampetch Paphungkorn</t>
+          <t>Micheal Ye</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>nampetch_pa@anantaraclub.com</t>
+          <t>mye@anantaraclub.com</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Nattaphat Petprom</t>
+          <t>Nagorn - ITALOT</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>nattaphat_pe@minor.com</t>
+          <t>nagorn@italots.com</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Oscar Lee</t>
+          <t>Nattaphat Petprom</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>wlee@minor.com</t>
+          <t>nattaphat_pe@minor.com</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1014,63 +1014,63 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Pak [CODEMONDAY] Aran T.</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>aran.t@codemonday.com</t>
+          <t>nikang@deloitte.com.cn</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Panachai</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>panachai_ch@anantaraclub.com</t>
+          <t>nyodkaew@deloitte.com</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Pasawish Imjumroon</t>
+          <t>Panachai</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>pasawish@italots.com</t>
+          <t>panachai_ch@anantaraclub.com</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>FS</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Pichalak Owchariyapitak</t>
+          <t>Pasawish Imjumroon</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>pichalak_ow@minor.com</t>
+          <t>pasawish@italots.com</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1082,46 +1082,46 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PIRAPOP THONGSANDEE</t>
+          <t>Oat - Marcom</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>pirapop_th@anantaraclub.com</t>
+          <t>pat_pa@minor.com</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>MarCom</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Pun</t>
+          <t xml:space="preserve">Pearploy </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>thamarak_kh@minor.com</t>
+          <t>pearploy_th@minor.com</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Commercial</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sahaschai Jiwakanon</t>
+          <t>Pichalak Owchariyapitak</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>sahaschai@italot.com</t>
+          <t>pichalak_ow@minor.com</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1133,165 +1133,165 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Samita Kongpanichkul</t>
+          <t>PIRAPOP THONGSANDEE</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>samita_ko@minor.com</t>
+          <t>pirapop_th@anantaraclub.com</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>FS</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sattaya Thomwan</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>sattaya_th@minor.com</t>
+          <t>pkeelawat@deloitte.com</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>sawittree_de</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>sawittree_de@anantaraclub.com</t>
+          <t>plertphati@deloitte.com</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sirawich Thanawich</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>sirawich@italot.com</t>
+          <t>psaejeam@deloitte.com</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Siwakiat Kanpattaranont</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>siwakiat@hypcode.co</t>
+          <t>pyordming@deloitte.com</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Suchakree_si</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>suchakree_si@minor.com</t>
+          <t>rbasheerahamed@deloitte.com</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Surawut Issarolarn</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>surawut_is@minor.com</t>
+          <t>rbundlukarn@deloitte.com</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tack [CODEMONDAY]</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>suparerk.y@codemonday.com</t>
+          <t>rogallagher@deloitte.com</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Thungong C</t>
+          <t>Sahaschai - ITALOT</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>thungong_ch@minor.com</t>
+          <t>sahaschai@italots.com</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Tichanon Sankham</t>
+          <t>Sattaya Thomwan</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>tichanon_sa@minor.com</t>
+          <t>sattaya_th@minor.com</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1303,12 +1303,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Tom√°s Bourgeois</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>tomas.bourgeois@arzion.com</t>
+          <t>shawcxiao@deloitte.com.cn</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1320,114 +1320,114 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Whachiravit Thanyathanachot</t>
+          <t>Win [CODEMONDAY]</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>whachiravit_th@minor.com</t>
+          <t>sittiporn.k@codemonday.com</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Win [CODEMONDAY]</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>sittiporn.k@codemonday.com</t>
+          <t>sjanklan@deloitte.com</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Wissaroot Samart</t>
+          <t>Bobby Leong</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>wissaroot_sa@minor.com</t>
+          <t>sleong@anantaraclub.com</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Lamai - Contract Admin</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>lamai_nu@minor.com</t>
+          <t>slikitphatham@deloitte.com</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Sahaschai - ITALOT</t>
+          <t>Andrew Ngan</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>sahaschai@italots.com</t>
+          <t>sngan@anantaraclub.com</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HHENG - Club</t>
+          <t>Suchakree_si</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>hheng@minor.com</t>
+          <t>suchakree_si@minor.com</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Woranat - ITALOT</t>
+          <t>Surawut Issarolarn</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>woranat@italots.com</t>
+          <t>surawut_is@minor.com</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1439,29 +1439,29 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pearploy </t>
+          <t>Thungong C</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>pearploy_th@minor.com</t>
+          <t>thungong_ch@minor.com</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Atiwit</t>
+          <t>Tichanon Sankham</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>atiwit_wi@minor.com</t>
+          <t>tichanon_sa@minor.com</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1473,80 +1473,80 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Arzion</t>
+          <t>Tom√°s Bourgeois</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>dario.pereyra@arzion.com</t>
+          <t>tomas.bourgeois@arzion.com</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Woranat</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>woranat_in@minor.com</t>
+          <t>tvivitvorn@deloitte.com</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Pichalak</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>pichalak_ow@anantaraclub.com</t>
+          <t>vping@deloitte.com.cn</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Club</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Apiwat</t>
+          <t>Whachiravit Thanyathanachot</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>apiwat.s@codemonday.com</t>
+          <t>whachiravit_th@minor.com</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Supanat</t>
+          <t>Wissaroot Samart</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>supanat@codemonday.com</t>
+          <t>wissaroot_sa@minor.com</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1558,183 +1558,34 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Deloitte</t>
+          <t>Oscar</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>tvivitvorn@deloitte.com</t>
+          <t>wlee@anantaraclub.com</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Club</t>
+          <t>MarCom</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Deloitte</t>
+          <t>Jasmine</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>nyodkaew@deloitte.com</t>
+          <t>yyeo@anantaraclub.com</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>slikitphatham@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>rbasheerahamed@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>gteo@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>pkeelawat@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Oat - Marcom</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>pat_pa@minor.com</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>pyordming@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Micheal Ye</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>mye@anantaraclub.com</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Deloitte</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>darchong@deloitte.com</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>thungong@thatwhy.me</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>IT</t>
         </is>
       </c>
     </row>

</xml_diff>